<commit_message>
updated with final work
</commit_message>
<xml_diff>
--- a/keeper.xlsx
+++ b/keeper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidthakur08/GitHub/fpl_explore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52BF53A-46E8-F244-930E-10C4CEC15EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F9D90F-B4B3-AE4A-AB55-41888DD3F008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{D128A629-7235-0B44-A5F8-CAAB19D686AA}"/>
   </bookViews>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DE77BE-27ED-1F42-B3D7-B8B63C96E7F3}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>